<commit_message>
Validaciones arregladas | Tabla
</commit_message>
<xml_diff>
--- a/ProyectoProgramacion/documento1.xlsx
+++ b/ProyectoProgramacion/documento1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ID</t>
   </si>
@@ -20,16 +20,10 @@
     <t>INFORMACION EXTRAIDA</t>
   </si>
   <si>
-    <t>empresa</t>
+    <t>aaa</t>
   </si>
   <si>
-    <t>Iansadro</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>2? lac Cnndes “antiano</t>
+    <t>Iansa</t>
   </si>
 </sst>
 </file>
@@ -80,7 +74,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -102,14 +96,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>